<commit_message>
Completed case report bias assessment
</commit_message>
<xml_diff>
--- a/input/raw_data/bias_assessment/case_report_bias_data_end.xlsx
+++ b/input/raw_data/bias_assessment/case_report_bias_data_end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/bias_assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{258A8366-0577-6F40-8705-2966E626FBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{47AC506B-5E48-E741-9892-D1B3E9CD8E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20560" yWindow="880" windowWidth="20580" windowHeight="12240" xr2:uid="{0EC282F7-924A-5B47-8692-5C057716A3B4}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="279">
   <si>
     <t>Study_ID</t>
   </si>
@@ -821,6 +821,42 @@
   </si>
   <si>
     <t>Lacking detail on physilogical and laboratory findings, but contains all data relevant to this study (apart from motivation).</t>
+  </si>
+  <si>
+    <t>Difficult to obtain individual medical history from case.</t>
+  </si>
+  <si>
+    <t>Demographic history lacking, but pertinent.</t>
+  </si>
+  <si>
+    <t>Lacks detail of post intervention outcome.</t>
+  </si>
+  <si>
+    <t>Lacking details on physical assessment, but other pertinent information contained within case report.</t>
+  </si>
+  <si>
+    <t>Assessment and condition not well described, but contains all information pertinent to this study.</t>
+  </si>
+  <si>
+    <t>Post intervention outcome not well described.</t>
+  </si>
+  <si>
+    <t>Post-intervention status not well documented, but no complications mentioned.</t>
+  </si>
+  <si>
+    <t>Doesn't elaborate on 'known psychiatric illness'.</t>
+  </si>
+  <si>
+    <t>Lacks detailed history and examination findings.</t>
+  </si>
+  <si>
+    <t>Lacks detail on physical assessment.</t>
+  </si>
+  <si>
+    <t>Lacks detail on outcome, but appears to be well as was hence admitted to psychiatry.</t>
+  </si>
+  <si>
+    <t>Diagnostics and physical assessment not well described, nor is surgical course or lessons learnt, but information relevant to this review contained.</t>
   </si>
 </sst>
 </file>
@@ -1688,8 +1724,8 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N151" sqref="N151"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N197" sqref="N197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8309,6 +8345,42 @@
       <c r="B151" t="s">
         <v>172</v>
       </c>
+      <c r="C151" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" t="s">
+        <v>13</v>
+      </c>
+      <c r="E151" t="s">
+        <v>13</v>
+      </c>
+      <c r="F151" t="s">
+        <v>13</v>
+      </c>
+      <c r="G151" t="s">
+        <v>13</v>
+      </c>
+      <c r="H151" t="s">
+        <v>13</v>
+      </c>
+      <c r="I151" t="s">
+        <v>13</v>
+      </c>
+      <c r="J151" t="s">
+        <v>13</v>
+      </c>
+      <c r="K151" t="s">
+        <v>15</v>
+      </c>
+      <c r="L151" t="s">
+        <v>16</v>
+      </c>
+      <c r="M151" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N151" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152">
@@ -8317,6 +8389,42 @@
       <c r="B152" t="s">
         <v>173</v>
       </c>
+      <c r="C152" t="s">
+        <v>13</v>
+      </c>
+      <c r="D152" t="s">
+        <v>13</v>
+      </c>
+      <c r="E152" t="s">
+        <v>13</v>
+      </c>
+      <c r="F152" t="s">
+        <v>13</v>
+      </c>
+      <c r="G152" t="s">
+        <v>13</v>
+      </c>
+      <c r="H152" t="s">
+        <v>13</v>
+      </c>
+      <c r="I152" t="s">
+        <v>13</v>
+      </c>
+      <c r="J152" t="s">
+        <v>13</v>
+      </c>
+      <c r="K152" t="s">
+        <v>15</v>
+      </c>
+      <c r="L152" t="s">
+        <v>16</v>
+      </c>
+      <c r="M152" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N152" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153">
@@ -8325,6 +8433,42 @@
       <c r="B153" t="s">
         <v>174</v>
       </c>
+      <c r="C153" t="s">
+        <v>13</v>
+      </c>
+      <c r="D153" t="s">
+        <v>13</v>
+      </c>
+      <c r="E153" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" t="s">
+        <v>13</v>
+      </c>
+      <c r="G153" t="s">
+        <v>13</v>
+      </c>
+      <c r="H153" t="s">
+        <v>13</v>
+      </c>
+      <c r="I153" t="s">
+        <v>13</v>
+      </c>
+      <c r="J153" t="s">
+        <v>13</v>
+      </c>
+      <c r="K153" t="s">
+        <v>15</v>
+      </c>
+      <c r="L153" t="s">
+        <v>16</v>
+      </c>
+      <c r="M153" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N153" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154">
@@ -8333,6 +8477,42 @@
       <c r="B154" t="s">
         <v>175</v>
       </c>
+      <c r="C154" t="s">
+        <v>13</v>
+      </c>
+      <c r="D154" t="s">
+        <v>13</v>
+      </c>
+      <c r="E154" t="s">
+        <v>13</v>
+      </c>
+      <c r="F154" t="s">
+        <v>13</v>
+      </c>
+      <c r="G154" t="s">
+        <v>13</v>
+      </c>
+      <c r="H154" t="s">
+        <v>13</v>
+      </c>
+      <c r="I154" t="s">
+        <v>13</v>
+      </c>
+      <c r="J154" t="s">
+        <v>13</v>
+      </c>
+      <c r="K154" t="s">
+        <v>15</v>
+      </c>
+      <c r="L154" t="s">
+        <v>16</v>
+      </c>
+      <c r="M154" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N154" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155">
@@ -8341,6 +8521,42 @@
       <c r="B155" t="s">
         <v>176</v>
       </c>
+      <c r="C155" t="s">
+        <v>13</v>
+      </c>
+      <c r="D155" t="s">
+        <v>13</v>
+      </c>
+      <c r="E155" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" t="s">
+        <v>13</v>
+      </c>
+      <c r="G155" t="s">
+        <v>13</v>
+      </c>
+      <c r="H155" t="s">
+        <v>13</v>
+      </c>
+      <c r="I155" t="s">
+        <v>13</v>
+      </c>
+      <c r="J155" t="s">
+        <v>13</v>
+      </c>
+      <c r="K155" t="s">
+        <v>15</v>
+      </c>
+      <c r="L155" t="s">
+        <v>16</v>
+      </c>
+      <c r="M155" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N155" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156">
@@ -8349,6 +8565,42 @@
       <c r="B156" t="s">
         <v>177</v>
       </c>
+      <c r="C156" t="s">
+        <v>13</v>
+      </c>
+      <c r="D156" t="s">
+        <v>13</v>
+      </c>
+      <c r="E156" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" t="s">
+        <v>13</v>
+      </c>
+      <c r="H156" t="s">
+        <v>13</v>
+      </c>
+      <c r="I156" t="s">
+        <v>13</v>
+      </c>
+      <c r="J156" t="s">
+        <v>13</v>
+      </c>
+      <c r="K156" t="s">
+        <v>15</v>
+      </c>
+      <c r="L156" t="s">
+        <v>16</v>
+      </c>
+      <c r="M156" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N156" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157">
@@ -8357,6 +8609,42 @@
       <c r="B157" t="s">
         <v>178</v>
       </c>
+      <c r="C157" t="s">
+        <v>13</v>
+      </c>
+      <c r="D157" t="s">
+        <v>13</v>
+      </c>
+      <c r="E157" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" t="s">
+        <v>13</v>
+      </c>
+      <c r="G157" t="s">
+        <v>13</v>
+      </c>
+      <c r="H157" t="s">
+        <v>13</v>
+      </c>
+      <c r="I157" t="s">
+        <v>13</v>
+      </c>
+      <c r="J157" t="s">
+        <v>13</v>
+      </c>
+      <c r="K157" t="s">
+        <v>15</v>
+      </c>
+      <c r="L157" t="s">
+        <v>16</v>
+      </c>
+      <c r="M157" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N157" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158">
@@ -8365,6 +8653,42 @@
       <c r="B158" t="s">
         <v>179</v>
       </c>
+      <c r="C158" t="s">
+        <v>13</v>
+      </c>
+      <c r="D158" t="s">
+        <v>13</v>
+      </c>
+      <c r="E158" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" t="s">
+        <v>13</v>
+      </c>
+      <c r="G158" t="s">
+        <v>13</v>
+      </c>
+      <c r="H158" t="s">
+        <v>13</v>
+      </c>
+      <c r="I158" t="s">
+        <v>13</v>
+      </c>
+      <c r="J158" t="s">
+        <v>13</v>
+      </c>
+      <c r="K158" t="s">
+        <v>15</v>
+      </c>
+      <c r="L158" t="s">
+        <v>16</v>
+      </c>
+      <c r="M158" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N158" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159">
@@ -8373,6 +8697,42 @@
       <c r="B159" t="s">
         <v>180</v>
       </c>
+      <c r="C159" t="s">
+        <v>13</v>
+      </c>
+      <c r="D159" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G159" t="s">
+        <v>13</v>
+      </c>
+      <c r="H159" t="s">
+        <v>13</v>
+      </c>
+      <c r="I159" t="s">
+        <v>13</v>
+      </c>
+      <c r="J159" t="s">
+        <v>13</v>
+      </c>
+      <c r="K159" t="s">
+        <v>15</v>
+      </c>
+      <c r="L159" t="s">
+        <v>16</v>
+      </c>
+      <c r="M159" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N159" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160">
@@ -8381,293 +8741,1625 @@
       <c r="B160" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C160" t="s">
+        <v>13</v>
+      </c>
+      <c r="D160" t="s">
+        <v>13</v>
+      </c>
+      <c r="E160" t="s">
+        <v>13</v>
+      </c>
+      <c r="F160" t="s">
+        <v>13</v>
+      </c>
+      <c r="G160" t="s">
+        <v>13</v>
+      </c>
+      <c r="H160" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" t="s">
+        <v>13</v>
+      </c>
+      <c r="J160" t="s">
+        <v>13</v>
+      </c>
+      <c r="K160" t="s">
+        <v>15</v>
+      </c>
+      <c r="L160" t="s">
+        <v>16</v>
+      </c>
+      <c r="M160" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N160" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>583</v>
       </c>
       <c r="B161" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C161" t="s">
+        <v>13</v>
+      </c>
+      <c r="D161" t="s">
+        <v>13</v>
+      </c>
+      <c r="E161" t="s">
+        <v>13</v>
+      </c>
+      <c r="F161" t="s">
+        <v>13</v>
+      </c>
+      <c r="G161" t="s">
+        <v>13</v>
+      </c>
+      <c r="H161" t="s">
+        <v>13</v>
+      </c>
+      <c r="I161" t="s">
+        <v>13</v>
+      </c>
+      <c r="J161" t="s">
+        <v>13</v>
+      </c>
+      <c r="K161" t="s">
+        <v>15</v>
+      </c>
+      <c r="L161" t="s">
+        <v>16</v>
+      </c>
+      <c r="M161" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N161" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>586</v>
       </c>
       <c r="B162" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C162" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" t="s">
+        <v>13</v>
+      </c>
+      <c r="E162" t="s">
+        <v>13</v>
+      </c>
+      <c r="F162" t="s">
+        <v>13</v>
+      </c>
+      <c r="G162" t="s">
+        <v>13</v>
+      </c>
+      <c r="H162" t="s">
+        <v>13</v>
+      </c>
+      <c r="I162" t="s">
+        <v>13</v>
+      </c>
+      <c r="J162" t="s">
+        <v>13</v>
+      </c>
+      <c r="K162" t="s">
+        <v>15</v>
+      </c>
+      <c r="L162" t="s">
+        <v>16</v>
+      </c>
+      <c r="M162" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N162" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>589</v>
       </c>
       <c r="B163" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C163" t="s">
+        <v>13</v>
+      </c>
+      <c r="D163" t="s">
+        <v>13</v>
+      </c>
+      <c r="E163" t="s">
+        <v>13</v>
+      </c>
+      <c r="F163" t="s">
+        <v>13</v>
+      </c>
+      <c r="G163" t="s">
+        <v>13</v>
+      </c>
+      <c r="H163" t="s">
+        <v>18</v>
+      </c>
+      <c r="I163" t="s">
+        <v>13</v>
+      </c>
+      <c r="J163" t="s">
+        <v>13</v>
+      </c>
+      <c r="K163" t="s">
+        <v>219</v>
+      </c>
+      <c r="L163" t="s">
+        <v>16</v>
+      </c>
+      <c r="M163" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N163" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>592</v>
       </c>
       <c r="B164" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C164" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" t="s">
+        <v>13</v>
+      </c>
+      <c r="F164" t="s">
+        <v>13</v>
+      </c>
+      <c r="G164" t="s">
+        <v>13</v>
+      </c>
+      <c r="H164" t="s">
+        <v>13</v>
+      </c>
+      <c r="I164" t="s">
+        <v>13</v>
+      </c>
+      <c r="J164" t="s">
+        <v>13</v>
+      </c>
+      <c r="K164" t="s">
+        <v>15</v>
+      </c>
+      <c r="L164" t="s">
+        <v>16</v>
+      </c>
+      <c r="M164" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N164" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>593</v>
       </c>
       <c r="B165" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C165" t="s">
+        <v>13</v>
+      </c>
+      <c r="D165" t="s">
+        <v>13</v>
+      </c>
+      <c r="E165" t="s">
+        <v>13</v>
+      </c>
+      <c r="F165" t="s">
+        <v>13</v>
+      </c>
+      <c r="G165" t="s">
+        <v>13</v>
+      </c>
+      <c r="H165" t="s">
+        <v>13</v>
+      </c>
+      <c r="I165" t="s">
+        <v>13</v>
+      </c>
+      <c r="J165" t="s">
+        <v>13</v>
+      </c>
+      <c r="K165" t="s">
+        <v>15</v>
+      </c>
+      <c r="L165" t="s">
+        <v>16</v>
+      </c>
+      <c r="M165" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N165" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>594</v>
       </c>
       <c r="B166" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C166" t="s">
+        <v>13</v>
+      </c>
+      <c r="D166" t="s">
+        <v>13</v>
+      </c>
+      <c r="E166" t="s">
+        <v>13</v>
+      </c>
+      <c r="F166" t="s">
+        <v>13</v>
+      </c>
+      <c r="G166" t="s">
+        <v>13</v>
+      </c>
+      <c r="H166" t="s">
+        <v>13</v>
+      </c>
+      <c r="I166" t="s">
+        <v>14</v>
+      </c>
+      <c r="J166" t="s">
+        <v>13</v>
+      </c>
+      <c r="K166" t="s">
+        <v>15</v>
+      </c>
+      <c r="L166" t="s">
+        <v>16</v>
+      </c>
+      <c r="M166" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N166" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>597</v>
       </c>
       <c r="B167" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C167" t="s">
+        <v>13</v>
+      </c>
+      <c r="D167" t="s">
+        <v>13</v>
+      </c>
+      <c r="E167" t="s">
+        <v>13</v>
+      </c>
+      <c r="F167" t="s">
+        <v>13</v>
+      </c>
+      <c r="G167" t="s">
+        <v>13</v>
+      </c>
+      <c r="H167" t="s">
+        <v>13</v>
+      </c>
+      <c r="I167" t="s">
+        <v>13</v>
+      </c>
+      <c r="J167" t="s">
+        <v>13</v>
+      </c>
+      <c r="K167" t="s">
+        <v>15</v>
+      </c>
+      <c r="L167" t="s">
+        <v>16</v>
+      </c>
+      <c r="M167" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N167" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>598</v>
       </c>
       <c r="B168" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C168" t="s">
+        <v>13</v>
+      </c>
+      <c r="D168" t="s">
+        <v>13</v>
+      </c>
+      <c r="E168" t="s">
+        <v>13</v>
+      </c>
+      <c r="F168" t="s">
+        <v>13</v>
+      </c>
+      <c r="G168" t="s">
+        <v>13</v>
+      </c>
+      <c r="H168" t="s">
+        <v>13</v>
+      </c>
+      <c r="I168" t="s">
+        <v>13</v>
+      </c>
+      <c r="J168" t="s">
+        <v>13</v>
+      </c>
+      <c r="K168" t="s">
+        <v>15</v>
+      </c>
+      <c r="L168" t="s">
+        <v>16</v>
+      </c>
+      <c r="M168" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N168" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>602</v>
       </c>
       <c r="B169" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C169" t="s">
+        <v>13</v>
+      </c>
+      <c r="D169" t="s">
+        <v>13</v>
+      </c>
+      <c r="E169" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" t="s">
+        <v>13</v>
+      </c>
+      <c r="G169" t="s">
+        <v>13</v>
+      </c>
+      <c r="H169" t="s">
+        <v>13</v>
+      </c>
+      <c r="I169" t="s">
+        <v>14</v>
+      </c>
+      <c r="J169" t="s">
+        <v>13</v>
+      </c>
+      <c r="K169" t="s">
+        <v>15</v>
+      </c>
+      <c r="L169" t="s">
+        <v>16</v>
+      </c>
+      <c r="M169" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N169" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>604</v>
       </c>
       <c r="B170" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C170" t="s">
+        <v>13</v>
+      </c>
+      <c r="D170" t="s">
+        <v>13</v>
+      </c>
+      <c r="E170" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" t="s">
+        <v>13</v>
+      </c>
+      <c r="G170" t="s">
+        <v>13</v>
+      </c>
+      <c r="H170" t="s">
+        <v>13</v>
+      </c>
+      <c r="I170" t="s">
+        <v>13</v>
+      </c>
+      <c r="J170" t="s">
+        <v>13</v>
+      </c>
+      <c r="K170" t="s">
+        <v>15</v>
+      </c>
+      <c r="L170" t="s">
+        <v>16</v>
+      </c>
+      <c r="M170" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N170" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>610</v>
       </c>
       <c r="B171" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D171" t="s">
+        <v>13</v>
+      </c>
+      <c r="E171" t="s">
+        <v>18</v>
+      </c>
+      <c r="F171" t="s">
+        <v>18</v>
+      </c>
+      <c r="G171" t="s">
+        <v>13</v>
+      </c>
+      <c r="H171" t="s">
+        <v>13</v>
+      </c>
+      <c r="I171" t="s">
+        <v>14</v>
+      </c>
+      <c r="J171" t="s">
+        <v>13</v>
+      </c>
+      <c r="K171" t="s">
+        <v>15</v>
+      </c>
+      <c r="L171" t="s">
+        <v>16</v>
+      </c>
+      <c r="M171" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N171" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>610</v>
       </c>
       <c r="B172" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C172" t="s">
+        <v>13</v>
+      </c>
+      <c r="D172" t="s">
+        <v>13</v>
+      </c>
+      <c r="E172" t="s">
+        <v>18</v>
+      </c>
+      <c r="F172" t="s">
+        <v>18</v>
+      </c>
+      <c r="G172" t="s">
+        <v>13</v>
+      </c>
+      <c r="H172" t="s">
+        <v>13</v>
+      </c>
+      <c r="I172" t="s">
+        <v>14</v>
+      </c>
+      <c r="J172" t="s">
+        <v>13</v>
+      </c>
+      <c r="K172" t="s">
+        <v>15</v>
+      </c>
+      <c r="L172" t="s">
+        <v>16</v>
+      </c>
+      <c r="M172" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N172" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>610</v>
       </c>
       <c r="B173" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C173" t="s">
+        <v>13</v>
+      </c>
+      <c r="D173" t="s">
+        <v>18</v>
+      </c>
+      <c r="E173" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" t="s">
+        <v>18</v>
+      </c>
+      <c r="G173" t="s">
+        <v>13</v>
+      </c>
+      <c r="H173" t="s">
+        <v>18</v>
+      </c>
+      <c r="I173" t="s">
+        <v>14</v>
+      </c>
+      <c r="J173" t="s">
+        <v>13</v>
+      </c>
+      <c r="K173" t="s">
+        <v>219</v>
+      </c>
+      <c r="L173" t="s">
+        <v>16</v>
+      </c>
+      <c r="M173" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N173" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>617</v>
       </c>
       <c r="B174" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C174" t="s">
+        <v>13</v>
+      </c>
+      <c r="D174" t="s">
+        <v>13</v>
+      </c>
+      <c r="E174" t="s">
+        <v>13</v>
+      </c>
+      <c r="F174" t="s">
+        <v>13</v>
+      </c>
+      <c r="G174" t="s">
+        <v>13</v>
+      </c>
+      <c r="H174" t="s">
+        <v>13</v>
+      </c>
+      <c r="I174" t="s">
+        <v>14</v>
+      </c>
+      <c r="J174" t="s">
+        <v>13</v>
+      </c>
+      <c r="K174" t="s">
+        <v>15</v>
+      </c>
+      <c r="L174" t="s">
+        <v>16</v>
+      </c>
+      <c r="M174" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N174" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>620</v>
       </c>
       <c r="B175" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C175" t="s">
+        <v>13</v>
+      </c>
+      <c r="D175" t="s">
+        <v>13</v>
+      </c>
+      <c r="E175" t="s">
+        <v>13</v>
+      </c>
+      <c r="F175" t="s">
+        <v>13</v>
+      </c>
+      <c r="G175" t="s">
+        <v>13</v>
+      </c>
+      <c r="H175" t="s">
+        <v>13</v>
+      </c>
+      <c r="I175" t="s">
+        <v>13</v>
+      </c>
+      <c r="J175" t="s">
+        <v>13</v>
+      </c>
+      <c r="K175" t="s">
+        <v>15</v>
+      </c>
+      <c r="L175" t="s">
+        <v>16</v>
+      </c>
+      <c r="M175" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N175" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>621</v>
       </c>
       <c r="B176" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C176" t="s">
+        <v>13</v>
+      </c>
+      <c r="D176" t="s">
+        <v>13</v>
+      </c>
+      <c r="E176" t="s">
+        <v>13</v>
+      </c>
+      <c r="F176" t="s">
+        <v>13</v>
+      </c>
+      <c r="G176" t="s">
+        <v>13</v>
+      </c>
+      <c r="H176" t="s">
+        <v>13</v>
+      </c>
+      <c r="I176" t="s">
+        <v>13</v>
+      </c>
+      <c r="J176" t="s">
+        <v>13</v>
+      </c>
+      <c r="K176" t="s">
+        <v>15</v>
+      </c>
+      <c r="L176" t="s">
+        <v>16</v>
+      </c>
+      <c r="M176" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N176" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>622</v>
       </c>
       <c r="B177" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C177" t="s">
+        <v>13</v>
+      </c>
+      <c r="D177" t="s">
+        <v>13</v>
+      </c>
+      <c r="E177" t="s">
+        <v>13</v>
+      </c>
+      <c r="F177" t="s">
+        <v>13</v>
+      </c>
+      <c r="G177" t="s">
+        <v>13</v>
+      </c>
+      <c r="H177" t="s">
+        <v>13</v>
+      </c>
+      <c r="I177" t="s">
+        <v>18</v>
+      </c>
+      <c r="J177" t="s">
+        <v>13</v>
+      </c>
+      <c r="K177" t="s">
+        <v>15</v>
+      </c>
+      <c r="L177" t="s">
+        <v>16</v>
+      </c>
+      <c r="M177" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N177" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>623</v>
       </c>
       <c r="B178" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C178" t="s">
+        <v>13</v>
+      </c>
+      <c r="D178" t="s">
+        <v>13</v>
+      </c>
+      <c r="E178" t="s">
+        <v>13</v>
+      </c>
+      <c r="F178" t="s">
+        <v>13</v>
+      </c>
+      <c r="G178" t="s">
+        <v>13</v>
+      </c>
+      <c r="H178" t="s">
+        <v>13</v>
+      </c>
+      <c r="I178" t="s">
+        <v>13</v>
+      </c>
+      <c r="J178" t="s">
+        <v>13</v>
+      </c>
+      <c r="K178" t="s">
+        <v>15</v>
+      </c>
+      <c r="L178" t="s">
+        <v>16</v>
+      </c>
+      <c r="M178" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N178" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>625</v>
       </c>
       <c r="B179" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C179" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179" t="s">
+        <v>13</v>
+      </c>
+      <c r="E179" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" t="s">
+        <v>13</v>
+      </c>
+      <c r="G179" t="s">
+        <v>13</v>
+      </c>
+      <c r="H179" t="s">
+        <v>13</v>
+      </c>
+      <c r="I179" t="s">
+        <v>14</v>
+      </c>
+      <c r="J179" t="s">
+        <v>13</v>
+      </c>
+      <c r="K179" t="s">
+        <v>15</v>
+      </c>
+      <c r="L179" t="s">
+        <v>16</v>
+      </c>
+      <c r="M179" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N179" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>626</v>
       </c>
       <c r="B180" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C180" t="s">
+        <v>13</v>
+      </c>
+      <c r="D180" t="s">
+        <v>13</v>
+      </c>
+      <c r="E180" t="s">
+        <v>13</v>
+      </c>
+      <c r="F180" t="s">
+        <v>13</v>
+      </c>
+      <c r="G180" t="s">
+        <v>13</v>
+      </c>
+      <c r="H180" t="s">
+        <v>13</v>
+      </c>
+      <c r="I180" t="s">
+        <v>13</v>
+      </c>
+      <c r="J180" t="s">
+        <v>13</v>
+      </c>
+      <c r="K180" t="s">
+        <v>15</v>
+      </c>
+      <c r="L180" t="s">
+        <v>16</v>
+      </c>
+      <c r="M180" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N180" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>637</v>
       </c>
       <c r="B181" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C181" t="s">
+        <v>13</v>
+      </c>
+      <c r="D181" t="s">
+        <v>13</v>
+      </c>
+      <c r="E181" t="s">
+        <v>13</v>
+      </c>
+      <c r="F181" t="s">
+        <v>13</v>
+      </c>
+      <c r="G181" t="s">
+        <v>13</v>
+      </c>
+      <c r="H181" t="s">
+        <v>13</v>
+      </c>
+      <c r="I181" t="s">
+        <v>13</v>
+      </c>
+      <c r="J181" t="s">
+        <v>13</v>
+      </c>
+      <c r="K181" t="s">
+        <v>15</v>
+      </c>
+      <c r="L181" t="s">
+        <v>16</v>
+      </c>
+      <c r="M181" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N181" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>640</v>
       </c>
       <c r="B182" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C182" t="s">
+        <v>13</v>
+      </c>
+      <c r="D182" t="s">
+        <v>13</v>
+      </c>
+      <c r="E182" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" t="s">
+        <v>13</v>
+      </c>
+      <c r="G182" t="s">
+        <v>13</v>
+      </c>
+      <c r="H182" t="s">
+        <v>13</v>
+      </c>
+      <c r="I182" t="s">
+        <v>13</v>
+      </c>
+      <c r="J182" t="s">
+        <v>13</v>
+      </c>
+      <c r="K182" t="s">
+        <v>15</v>
+      </c>
+      <c r="L182" t="s">
+        <v>16</v>
+      </c>
+      <c r="M182" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N182" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>643</v>
       </c>
       <c r="B183" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C183" t="s">
+        <v>13</v>
+      </c>
+      <c r="D183" t="s">
+        <v>13</v>
+      </c>
+      <c r="E183" t="s">
+        <v>13</v>
+      </c>
+      <c r="F183" t="s">
+        <v>13</v>
+      </c>
+      <c r="G183" t="s">
+        <v>13</v>
+      </c>
+      <c r="H183" t="s">
+        <v>13</v>
+      </c>
+      <c r="I183" t="s">
+        <v>18</v>
+      </c>
+      <c r="J183" t="s">
+        <v>13</v>
+      </c>
+      <c r="K183" t="s">
+        <v>15</v>
+      </c>
+      <c r="L183" t="s">
+        <v>16</v>
+      </c>
+      <c r="M183" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N183" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>644</v>
       </c>
       <c r="B184" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C184" t="s">
+        <v>13</v>
+      </c>
+      <c r="D184" t="s">
+        <v>13</v>
+      </c>
+      <c r="E184" t="s">
+        <v>13</v>
+      </c>
+      <c r="F184" t="s">
+        <v>13</v>
+      </c>
+      <c r="G184" t="s">
+        <v>13</v>
+      </c>
+      <c r="H184" t="s">
+        <v>13</v>
+      </c>
+      <c r="I184" t="s">
+        <v>13</v>
+      </c>
+      <c r="J184" t="s">
+        <v>13</v>
+      </c>
+      <c r="K184" t="s">
+        <v>15</v>
+      </c>
+      <c r="L184" t="s">
+        <v>16</v>
+      </c>
+      <c r="M184" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N184" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>651</v>
       </c>
       <c r="B185" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C185" t="s">
+        <v>13</v>
+      </c>
+      <c r="D185" t="s">
+        <v>13</v>
+      </c>
+      <c r="E185" t="s">
+        <v>13</v>
+      </c>
+      <c r="F185" t="s">
+        <v>13</v>
+      </c>
+      <c r="G185" t="s">
+        <v>13</v>
+      </c>
+      <c r="H185" t="s">
+        <v>13</v>
+      </c>
+      <c r="I185" t="s">
+        <v>14</v>
+      </c>
+      <c r="J185" t="s">
+        <v>13</v>
+      </c>
+      <c r="K185" t="s">
+        <v>15</v>
+      </c>
+      <c r="L185" t="s">
+        <v>16</v>
+      </c>
+      <c r="M185" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N185" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>652</v>
       </c>
       <c r="B186" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C186" t="s">
+        <v>13</v>
+      </c>
+      <c r="D186" t="s">
+        <v>13</v>
+      </c>
+      <c r="E186" t="s">
+        <v>13</v>
+      </c>
+      <c r="F186" t="s">
+        <v>13</v>
+      </c>
+      <c r="G186" t="s">
+        <v>13</v>
+      </c>
+      <c r="H186" t="s">
+        <v>13</v>
+      </c>
+      <c r="I186" t="s">
+        <v>13</v>
+      </c>
+      <c r="J186" t="s">
+        <v>13</v>
+      </c>
+      <c r="K186" t="s">
+        <v>15</v>
+      </c>
+      <c r="L186" t="s">
+        <v>16</v>
+      </c>
+      <c r="M186" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N186" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>654</v>
       </c>
       <c r="B187" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D187" t="s">
+        <v>13</v>
+      </c>
+      <c r="E187" t="s">
+        <v>13</v>
+      </c>
+      <c r="F187" t="s">
+        <v>13</v>
+      </c>
+      <c r="G187" t="s">
+        <v>13</v>
+      </c>
+      <c r="H187" t="s">
+        <v>13</v>
+      </c>
+      <c r="I187" t="s">
+        <v>13</v>
+      </c>
+      <c r="J187" t="s">
+        <v>13</v>
+      </c>
+      <c r="K187" t="s">
+        <v>15</v>
+      </c>
+      <c r="L187" t="s">
+        <v>16</v>
+      </c>
+      <c r="M187" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N187" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>658</v>
       </c>
       <c r="B188" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C188" t="s">
+        <v>13</v>
+      </c>
+      <c r="D188" t="s">
+        <v>18</v>
+      </c>
+      <c r="E188" t="s">
+        <v>13</v>
+      </c>
+      <c r="F188" t="s">
+        <v>18</v>
+      </c>
+      <c r="G188" t="s">
+        <v>13</v>
+      </c>
+      <c r="H188" t="s">
+        <v>13</v>
+      </c>
+      <c r="I188" t="s">
+        <v>14</v>
+      </c>
+      <c r="J188" t="s">
+        <v>18</v>
+      </c>
+      <c r="K188" t="s">
+        <v>15</v>
+      </c>
+      <c r="L188" t="s">
+        <v>16</v>
+      </c>
+      <c r="M188" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N188" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>661</v>
       </c>
       <c r="B189" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C189" t="s">
+        <v>13</v>
+      </c>
+      <c r="D189" t="s">
+        <v>13</v>
+      </c>
+      <c r="E189" t="s">
+        <v>13</v>
+      </c>
+      <c r="F189" t="s">
+        <v>13</v>
+      </c>
+      <c r="G189" t="s">
+        <v>13</v>
+      </c>
+      <c r="H189" t="s">
+        <v>13</v>
+      </c>
+      <c r="I189" t="s">
+        <v>13</v>
+      </c>
+      <c r="J189" t="s">
+        <v>13</v>
+      </c>
+      <c r="K189" t="s">
+        <v>15</v>
+      </c>
+      <c r="L189" t="s">
+        <v>16</v>
+      </c>
+      <c r="M189" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N189" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>667</v>
       </c>
       <c r="B190" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C190" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" t="s">
+        <v>13</v>
+      </c>
+      <c r="E190" t="s">
+        <v>13</v>
+      </c>
+      <c r="F190" t="s">
+        <v>13</v>
+      </c>
+      <c r="G190" t="s">
+        <v>13</v>
+      </c>
+      <c r="H190" t="s">
+        <v>13</v>
+      </c>
+      <c r="I190" t="s">
+        <v>14</v>
+      </c>
+      <c r="J190" t="s">
+        <v>13</v>
+      </c>
+      <c r="K190" t="s">
+        <v>15</v>
+      </c>
+      <c r="L190" t="s">
+        <v>16</v>
+      </c>
+      <c r="M190" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N190" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>675</v>
       </c>
       <c r="B191" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C191" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" t="s">
+        <v>13</v>
+      </c>
+      <c r="F191" t="s">
+        <v>13</v>
+      </c>
+      <c r="G191" t="s">
+        <v>13</v>
+      </c>
+      <c r="H191" t="s">
+        <v>13</v>
+      </c>
+      <c r="I191" t="s">
+        <v>14</v>
+      </c>
+      <c r="J191" t="s">
+        <v>13</v>
+      </c>
+      <c r="K191" t="s">
+        <v>15</v>
+      </c>
+      <c r="L191" t="s">
+        <v>16</v>
+      </c>
+      <c r="M191" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N191" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>680</v>
       </c>
       <c r="B192" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C192" t="s">
+        <v>13</v>
+      </c>
+      <c r="D192" t="s">
+        <v>13</v>
+      </c>
+      <c r="E192" t="s">
+        <v>13</v>
+      </c>
+      <c r="F192" t="s">
+        <v>13</v>
+      </c>
+      <c r="G192" t="s">
+        <v>13</v>
+      </c>
+      <c r="H192" t="s">
+        <v>13</v>
+      </c>
+      <c r="I192" t="s">
+        <v>14</v>
+      </c>
+      <c r="J192" t="s">
+        <v>13</v>
+      </c>
+      <c r="K192" t="s">
+        <v>15</v>
+      </c>
+      <c r="L192" t="s">
+        <v>16</v>
+      </c>
+      <c r="M192" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N192" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>683</v>
       </c>
       <c r="B193" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C193" t="s">
+        <v>13</v>
+      </c>
+      <c r="D193" t="s">
+        <v>13</v>
+      </c>
+      <c r="E193" t="s">
+        <v>13</v>
+      </c>
+      <c r="F193" t="s">
+        <v>13</v>
+      </c>
+      <c r="G193" t="s">
+        <v>13</v>
+      </c>
+      <c r="H193" t="s">
+        <v>13</v>
+      </c>
+      <c r="I193" t="s">
+        <v>13</v>
+      </c>
+      <c r="J193" t="s">
+        <v>13</v>
+      </c>
+      <c r="K193" t="s">
+        <v>15</v>
+      </c>
+      <c r="L193" t="s">
+        <v>16</v>
+      </c>
+      <c r="M193" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N193" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>684</v>
       </c>
       <c r="B194" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C194" t="s">
+        <v>13</v>
+      </c>
+      <c r="D194" t="s">
+        <v>13</v>
+      </c>
+      <c r="E194" t="s">
+        <v>13</v>
+      </c>
+      <c r="F194" t="s">
+        <v>13</v>
+      </c>
+      <c r="G194" t="s">
+        <v>13</v>
+      </c>
+      <c r="H194" t="s">
+        <v>13</v>
+      </c>
+      <c r="I194" t="s">
+        <v>14</v>
+      </c>
+      <c r="J194" t="s">
+        <v>13</v>
+      </c>
+      <c r="K194" t="s">
+        <v>15</v>
+      </c>
+      <c r="L194" t="s">
+        <v>16</v>
+      </c>
+      <c r="M194" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N194" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>686</v>
       </c>
       <c r="B195" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C195" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" t="s">
+        <v>13</v>
+      </c>
+      <c r="F195" t="s">
+        <v>13</v>
+      </c>
+      <c r="G195" t="s">
+        <v>13</v>
+      </c>
+      <c r="H195" t="s">
+        <v>13</v>
+      </c>
+      <c r="I195" t="s">
+        <v>14</v>
+      </c>
+      <c r="J195" t="s">
+        <v>13</v>
+      </c>
+      <c r="K195" t="s">
+        <v>15</v>
+      </c>
+      <c r="L195" t="s">
+        <v>16</v>
+      </c>
+      <c r="M195" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N195" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>692</v>
       </c>
       <c r="B196" t="s">
         <v>217</v>
+      </c>
+      <c r="C196" t="s">
+        <v>13</v>
+      </c>
+      <c r="D196" t="s">
+        <v>13</v>
+      </c>
+      <c r="E196" t="s">
+        <v>13</v>
+      </c>
+      <c r="F196" t="s">
+        <v>13</v>
+      </c>
+      <c r="G196" t="s">
+        <v>13</v>
+      </c>
+      <c r="H196" t="s">
+        <v>13</v>
+      </c>
+      <c r="I196" t="s">
+        <v>14</v>
+      </c>
+      <c r="J196" t="s">
+        <v>13</v>
+      </c>
+      <c r="K196" t="s">
+        <v>15</v>
+      </c>
+      <c r="L196" t="s">
+        <v>16</v>
+      </c>
+      <c r="M196" s="2">
+        <v>45790</v>
+      </c>
+      <c r="N196" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="1048576" spans="13:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Commenced case series data extraction
</commit_message>
<xml_diff>
--- a/input/raw_data/bias_assessment/case_report_bias_data_end.xlsx
+++ b/input/raw_data/bias_assessment/case_report_bias_data_end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/bias_assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{08C627C4-6A30-F64D-921F-7471990BCD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0284D0BF-F37C-9943-BA95-BE4E58A20924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20560" yWindow="880" windowWidth="20580" windowHeight="12240" xr2:uid="{0EC282F7-924A-5B47-8692-5C057716A3B4}"/>
   </bookViews>
@@ -1724,8 +1724,8 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:L1"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>